<commit_message>
fix date of email sent
</commit_message>
<xml_diff>
--- a/leads.xlsx
+++ b/leads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresreality/Documents/crmai/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0E3373-FA4F-8840-BFAA-057C0317CED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D686B9-A179-C546-AFD8-5DF8722993D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="96">
   <si>
     <t>Position</t>
   </si>
@@ -151,6 +151,9 @@
     <t>Days Until Next Action</t>
   </si>
   <si>
+    <t>Last Action Date</t>
+  </si>
+  <si>
     <t>Joint CEO</t>
   </si>
   <si>
@@ -179,6 +182,9 @@
   </si>
   <si>
     <t>WooCommerce</t>
+  </si>
+  <si>
+    <t>2025-03-24</t>
   </si>
   <si>
     <t>Chief Financial Officer</t>
@@ -669,21 +675,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ8"/>
+  <dimension ref="A1:AR8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="14" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="24.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -813,37 +817,40 @@
       <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N2" s="2">
         <v>45739</v>
@@ -854,6 +861,7 @@
       <c r="Q2" t="s">
         <v>8</v>
       </c>
+      <c r="R2" s="2"/>
       <c r="AN2">
         <v>1</v>
       </c>
@@ -866,37 +874,40 @@
       <c r="AQ2">
         <v>0</v>
       </c>
+      <c r="AR2" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" t="s">
         <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K3" t="s">
-        <v>52</v>
       </c>
       <c r="N3" s="2">
         <v>45734</v>
@@ -905,7 +916,7 @@
         <v>45734</v>
       </c>
       <c r="Q3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R3" s="2">
         <v>45736</v>
@@ -926,36 +937,36 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N4" s="2">
         <v>45735</v>
@@ -964,7 +975,7 @@
         <v>45734</v>
       </c>
       <c r="Q4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R4" s="2">
         <v>45735</v>
@@ -979,10 +990,10 @@
         <v>8</v>
       </c>
       <c r="W4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AM4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AN4">
         <v>5</v>
@@ -997,36 +1008,36 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N5" s="2">
         <v>45739</v>
@@ -1034,6 +1045,9 @@
       <c r="Q5" t="s">
         <v>8</v>
       </c>
+      <c r="R5" s="2">
+        <v>45740</v>
+      </c>
       <c r="AN5">
         <v>1</v>
       </c>
@@ -1046,37 +1060,40 @@
       <c r="AQ5">
         <v>0</v>
       </c>
+      <c r="AR5" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="K6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N6" s="2">
         <v>45734</v>
@@ -1091,7 +1108,7 @@
         <v>45735</v>
       </c>
       <c r="S6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T6" s="2">
         <v>45736</v>
@@ -1100,7 +1117,7 @@
         <v>8</v>
       </c>
       <c r="W6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AN6">
         <v>6</v>
@@ -1115,33 +1132,33 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="K7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N7" s="2">
         <v>45734</v>
@@ -1156,7 +1173,7 @@
         <v>45735</v>
       </c>
       <c r="S7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T7" s="2">
         <v>45736</v>
@@ -1165,7 +1182,7 @@
         <v>8</v>
       </c>
       <c r="W7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AN7">
         <v>6</v>
@@ -1180,36 +1197,36 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" t="s">
         <v>93</v>
       </c>
-      <c r="F8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G8" t="s">
-        <v>89</v>
-      </c>
-      <c r="I8" t="s">
-        <v>90</v>
-      </c>
-      <c r="J8" t="s">
-        <v>91</v>
-      </c>
       <c r="K8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N8" s="2">
         <v>45734</v>
@@ -1224,7 +1241,7 @@
         <v>45735</v>
       </c>
       <c r="S8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T8" s="2">
         <v>45736</v>
@@ -1233,7 +1250,7 @@
         <v>8</v>
       </c>
       <c r="W8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AN8">
         <v>6</v>

</xml_diff>

<commit_message>
update dates for emails and count
</commit_message>
<xml_diff>
--- a/leads.xlsx
+++ b/leads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresreality/Documents/crmai/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D686B9-A179-C546-AFD8-5DF8722993D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562F32D0-33E2-2545-9D10-1955F47E2AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="97">
   <si>
     <t>Position</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>Last Action Date</t>
+  </si>
+  <si>
+    <t>Emails Sent Count</t>
   </si>
   <si>
     <t>Joint CEO</t>
@@ -675,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR8"/>
+  <dimension ref="A1:AS8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -687,7 +690,7 @@
     <col min="20" max="20" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -820,37 +823,40 @@
       <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N2" s="2">
         <v>45739</v>
@@ -875,39 +881,42 @@
         <v>0</v>
       </c>
       <c r="AR2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AS2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" t="s">
-        <v>53</v>
       </c>
       <c r="N3" s="2">
         <v>45734</v>
@@ -916,7 +925,7 @@
         <v>45734</v>
       </c>
       <c r="Q3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R3" s="2">
         <v>45736</v>
@@ -936,37 +945,40 @@
       <c r="AQ3">
         <v>-2</v>
       </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N4" s="2">
         <v>45735</v>
@@ -975,7 +987,7 @@
         <v>45734</v>
       </c>
       <c r="Q4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R4" s="2">
         <v>45735</v>
@@ -990,10 +1002,10 @@
         <v>8</v>
       </c>
       <c r="W4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AM4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AN4">
         <v>5</v>
@@ -1007,37 +1019,40 @@
       <c r="AQ4">
         <v>-1</v>
       </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N5" s="2">
         <v>45739</v>
@@ -1061,39 +1076,42 @@
         <v>0</v>
       </c>
       <c r="AR5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AS5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G6" t="s">
-        <v>91</v>
-      </c>
-      <c r="I6" t="s">
-        <v>92</v>
-      </c>
-      <c r="J6" t="s">
-        <v>93</v>
-      </c>
-      <c r="K6" t="s">
-        <v>53</v>
       </c>
       <c r="N6" s="2">
         <v>45734</v>
@@ -1108,7 +1126,7 @@
         <v>45735</v>
       </c>
       <c r="S6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="T6" s="2">
         <v>45736</v>
@@ -1117,7 +1135,7 @@
         <v>8</v>
       </c>
       <c r="W6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AN6">
         <v>6</v>
@@ -1131,34 +1149,37 @@
       <c r="AQ6">
         <v>-2</v>
       </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" t="s">
         <v>94</v>
       </c>
-      <c r="F7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J7" t="s">
-        <v>93</v>
-      </c>
       <c r="K7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N7" s="2">
         <v>45734</v>
@@ -1173,7 +1194,7 @@
         <v>45735</v>
       </c>
       <c r="S7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="T7" s="2">
         <v>45736</v>
@@ -1182,7 +1203,7 @@
         <v>8</v>
       </c>
       <c r="W7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AN7">
         <v>6</v>
@@ -1196,37 +1217,40 @@
       <c r="AQ7">
         <v>-2</v>
       </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N8" s="2">
         <v>45734</v>
@@ -1241,7 +1265,7 @@
         <v>45735</v>
       </c>
       <c r="S8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="T8" s="2">
         <v>45736</v>
@@ -1250,7 +1274,7 @@
         <v>8</v>
       </c>
       <c r="W8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AN8">
         <v>6</v>
@@ -1263,6 +1287,9 @@
       </c>
       <c r="AQ8">
         <v>-2</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
forgot if i added
</commit_message>
<xml_diff>
--- a/leads.xlsx
+++ b/leads.xlsx
@@ -490,7 +490,7 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Calls</t>
+          <t>Technology</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -500,7 +500,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Technology</t>
+          <t>Technology.1</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">

</xml_diff>